<commit_message>
added selections and seedlots
</commit_message>
<xml_diff>
--- a/data/Cornell_WinterOatPeaIntercrop_2024_Ithaca_plot_meta.xlsx
+++ b/data/Cornell_WinterOatPeaIntercrop_2024_Ithaca_plot_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2024_winter\2024_winter_intercrop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F2FCE2-C8ED-45EE-95A6-893B77A4E198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D0D20C-745E-4692-B681-849E626BF8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FD46450C-E646-4132-9981-A5248A9FD285}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="21270" xr2:uid="{FD46450C-E646-4132-9981-A5248A9FD285}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>